<commit_message>
tangy bitter gourd, updates in weekly menu and template
</commit_message>
<xml_diff>
--- a/Recipe template.xlsx
+++ b/Recipe template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\Google Drive\recipies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitkumar/Dropbox/recipies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA1A8E-A6E4-4C58-9B39-3887FBA1602D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64734C86-0691-8946-9DD9-E092D634DB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{134C7825-DF8B-42D3-A51C-71C91B0E6488}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{134C7825-DF8B-42D3-A51C-71C91B0E6488}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,23 +498,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E1998A-25FC-42BE-BFFC-DAF05717235E}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <f t="shared" ref="B3:B24" si="0">(E3/F3)*D3</f>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5">
         <f t="shared" si="0"/>
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5">
         <f t="shared" si="0"/>
@@ -593,7 +593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5">
         <f t="shared" si="0"/>
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5">
         <f t="shared" si="0"/>
@@ -632,7 +632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5">
         <f t="shared" si="0"/>
@@ -650,7 +650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5">
         <f t="shared" si="0"/>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
@@ -683,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5">
         <f t="shared" si="0"/>
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5">
         <f t="shared" si="0"/>
@@ -716,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5">
         <f t="shared" si="0"/>
@@ -731,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5">
         <f t="shared" si="0"/>
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5">
         <f t="shared" si="0"/>
@@ -776,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5">
         <f t="shared" si="0"/>
@@ -791,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="5">
         <f t="shared" si="0"/>
@@ -806,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5">
         <f t="shared" si="0"/>
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="5">
         <f t="shared" si="0"/>
@@ -836,7 +836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5">
         <f t="shared" si="0"/>
@@ -851,7 +851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="5">
         <f t="shared" si="0"/>
@@ -866,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5">
         <f t="shared" si="0"/>
@@ -881,7 +881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="5">
         <f t="shared" si="0"/>

</xml_diff>